<commit_message>
TCCP: Really fix speed bump Cypress tests
</commit_message>
<xml_diff>
--- a/cfgov/tccp/tests/data/sample.xlsx
+++ b/cfgov/tccp/tests/data/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chosaka/Projects/consumerfinance.gov/cfgov/tccp/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768ABAC4-841D-2F49-859C-FC66C5D4D6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE22D2D2-7C2C-0744-904E-8A2EB0DDBFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="520" windowWidth="27640" windowHeight="16940" xr2:uid="{773B7478-5D1D-1D4B-9B29-3632882A4CFE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="180">
   <si>
     <t>Notes</t>
   </si>
@@ -573,6 +573,12 @@
   </si>
   <si>
     <t>Other rewards</t>
+  </si>
+  <si>
+    <t>SAMPLE MIDWEST</t>
+  </si>
+  <si>
+    <t>Sample Fun Card</t>
   </si>
 </sst>
 </file>
@@ -697,7 +703,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -762,12 +768,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD5D3D1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -799,6 +814,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1114,11 +1135,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069A179E-C136-504D-90A5-5755E53482D8}">
-  <dimension ref="A1:FT15"/>
+  <dimension ref="A1:FT16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3515,7 +3534,91 @@
       </c>
       <c r="FO14" s="22"/>
     </row>
-    <row r="15" spans="1:176" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:176" x14ac:dyDescent="0.2">
+      <c r="A15" s="13"/>
+      <c r="B15" t="s">
+        <v>178</v>
+      </c>
+      <c r="C15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D15" s="28">
+        <v>44926</v>
+      </c>
+      <c r="E15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="N15" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="O15" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="P15" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>122</v>
+      </c>
+      <c r="R15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="AH15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="AI15">
+        <v>9.99</v>
+      </c>
+      <c r="AJ15">
+        <v>6.99</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>122</v>
+      </c>
+      <c r="AW15" t="s">
+        <v>122</v>
+      </c>
+      <c r="BG15" t="s">
+        <v>122</v>
+      </c>
+      <c r="BO15" t="s">
+        <v>122</v>
+      </c>
+      <c r="BQ15" t="s">
+        <v>122</v>
+      </c>
+      <c r="BS15" t="s">
+        <v>124</v>
+      </c>
+      <c r="CF15" t="s">
+        <v>122</v>
+      </c>
+      <c r="CL15" t="s">
+        <v>122</v>
+      </c>
+      <c r="CR15" t="s">
+        <v>122</v>
+      </c>
+      <c r="CY15" t="s">
+        <v>122</v>
+      </c>
+      <c r="DE15" t="s">
+        <v>122</v>
+      </c>
+      <c r="DN15" t="s">
+        <v>122</v>
+      </c>
+      <c r="DR15" t="s">
+        <v>122</v>
+      </c>
+      <c r="EO15" t="s">
+        <v>175</v>
+      </c>
+      <c r="FO15" s="22"/>
+    </row>
+    <row r="16" spans="1:176" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A10:FT13" xr:uid="{069A179E-C136-504D-90A5-5755E53482D8}"/>
   <phoneticPr fontId="11" type="noConversion"/>

</xml_diff>